<commit_message>
EMA list update to include more fields
</commit_message>
<xml_diff>
--- a/merge_fda_ema_pmda/force_merge_fields.xlsx
+++ b/merge_fda_ema_pmda/force_merge_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdeluca/Research/Postdoc/ARPA-H/Matrix_repos/matrix-drug-list/merge_fda_ema_pmda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D73396-81AF-A240-8091-4BAE3FE998EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CED590-4A67-8E43-816D-1DC4DD7F4FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{546DCC8F-AE7E-4C48-B286-70D7056F6CFB}"/>
   </bookViews>
@@ -36,12 +36,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Field to Keep</t>
   </si>
   <si>
     <t>Field to Remove</t>
+  </si>
+  <si>
+    <t>AGALSIDASE BETA</t>
+  </si>
+  <si>
+    <t>AGALSIDASE BETA  [AGALSIDASE BETA BIOSIMILAR 1]</t>
+  </si>
+  <si>
+    <t>ALENDRONATE SODIUM HYDRATE</t>
+  </si>
+  <si>
+    <t>ALENDRONATE SODIUM</t>
+  </si>
+  <si>
+    <t>AMLODIPINE BESILATE</t>
+  </si>
+  <si>
+    <t>AMLODIPINE BESYLATE</t>
+  </si>
+  <si>
+    <t>AMLODIPINE BESILATE; ATORVASTATIN CALCIUM HYDRATE</t>
+  </si>
+  <si>
+    <t>AMLODIPINE BESYLATE; ATORVASTATIN CALCIUM</t>
+  </si>
+  <si>
+    <t>AMLODIPINE BESYLATE; VALSARTAN</t>
+  </si>
+  <si>
+    <t>AMLODIPINE, VALSARTAN</t>
+  </si>
+  <si>
+    <t>ANAGRELIDE HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>ANAGRELIDE HYDROCHLORIDE HYDRATE</t>
+  </si>
+  <si>
+    <t>APOMORPHINE HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>APOMORPHINE HYDROCHLORIDE HYDRATE</t>
+  </si>
+  <si>
+    <t>ARGATROBAN</t>
+  </si>
+  <si>
+    <t>ARGATROBAN HYDRATE</t>
+  </si>
+  <si>
+    <t>BELUMOSUDIL MESILATE</t>
+  </si>
+  <si>
+    <t>BELUMOSUDIL MESYLATE</t>
+  </si>
+  <si>
+    <t>BETAINE</t>
+  </si>
+  <si>
+    <t>BETAINE ANHYDROUS</t>
+  </si>
+  <si>
+    <t>BOSENTAN</t>
+  </si>
+  <si>
+    <t>BOSENTAN HYDRATE</t>
+  </si>
+  <si>
+    <t>BOSENTAN MONOHYDRATE</t>
+  </si>
+  <si>
+    <t>BOSUTINIB</t>
+  </si>
+  <si>
+    <t>BOSUTINIB HYDRATE</t>
+  </si>
+  <si>
+    <t>BOSUTINIB MONOHYDRATE</t>
+  </si>
+  <si>
+    <t>BUDESONIDE; FORMOTEROL FUMARATE</t>
+  </si>
+  <si>
+    <t>BUDESONIDE; FORMOTEROL FUMARATE DIHYDRATE</t>
+  </si>
+  <si>
+    <t>BUDESONIDE; FORMOTEROL FUMARATE HYDRATE</t>
+  </si>
+  <si>
+    <t>CANAGLIFLOZIN</t>
+  </si>
+  <si>
+    <t>CANAGLIFLOZIN HYDRATE</t>
+  </si>
+  <si>
+    <t>CAPMATINIB HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>CAPMATINIB HYDROCHLORIDE HYDRATE</t>
+  </si>
+  <si>
+    <t>CASIRIVIMAB, IMDEVIMAB</t>
+  </si>
+  <si>
+    <t>CASIRIVIMAB; IMDEVIMAB</t>
+  </si>
+  <si>
+    <t>CEFEPIME DIHYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>CEFEPIME HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>CEFIDEROCOL SULFATE TOSYLATE</t>
+  </si>
+  <si>
+    <t>CEFIDEROCOL TOSILATE SULFATE HYDRATE</t>
   </si>
 </sst>
 </file>
@@ -431,7 +548,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B60"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,7 +565,175 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
     </row>
   </sheetData>

</xml_diff>